<commit_message>
saving figures in pdf (vector)
</commit_message>
<xml_diff>
--- a/output/results_dblp_imdb_fnn_bnn_emb_nns.xlsx
+++ b/output/results_dblp_imdb_fnn_bnn_emb_nns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Github\Fani-Lab\neural_team_formation\dblp\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE99FB02-60B3-4189-9C6A-5A12A0E3797F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{137FC677-6B9D-4772-A34A-60EFC91DCB81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DBLP" sheetId="2" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="103">
   <si>
     <t>dblp-fnn-nons</t>
   </si>
@@ -742,7 +742,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -912,6 +912,15 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -936,15 +945,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -24355,6 +24378,307 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'IMDB-Efficiency'!$G$11:$G$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.48794535666595901</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.615988630382029</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.51841890253016698</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.51439078819994</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.510182913996448</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.48306082604941802</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.45633047297151802</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.49614977318761799</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1D64-4C53-83AF-13F4E579F8F9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="750823744"/>
+        <c:axId val="750830400"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="750823744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="750830400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="750830400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="750823744"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
@@ -32994,6 +33318,46 @@
 </file>
 
 <file path=xl/charts/colors12.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors13.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -34891,6 +35255,522 @@
 </file>
 
 <file path=xl/charts/style12.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style13.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -40223,6 +41103,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>679174</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>86139</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>389283</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>13252</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0369C9C5-77DD-46CE-8FB5-CFC0BB0DEABF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -42036,10 +42952,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE483F02-EABB-410C-B581-D071545F3EF7}">
-  <dimension ref="A1:AO64"/>
+  <dimension ref="A1:AI64"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47:O47"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -42058,37 +42974,38 @@
     <col min="21" max="22" width="7" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="8" bestFit="1" customWidth="1"/>
     <col min="24" max="28" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="C1" s="103" t="s">
+      <c r="C1" s="96" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="103"/>
-      <c r="G1" s="103"/>
-      <c r="H1" s="103"/>
-      <c r="I1" s="103"/>
-      <c r="J1" s="103"/>
-      <c r="K1" s="103"/>
-      <c r="L1" s="103"/>
-      <c r="M1" s="103"/>
-      <c r="N1" s="104"/>
-      <c r="O1" s="103" t="s">
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="J1" s="96"/>
+      <c r="K1" s="96"/>
+      <c r="L1" s="96"/>
+      <c r="M1" s="96"/>
+      <c r="N1" s="97"/>
+      <c r="O1" s="96" t="s">
         <v>56</v>
       </c>
-      <c r="P1" s="103"/>
-      <c r="Q1" s="103"/>
-      <c r="R1" s="103"/>
-      <c r="S1" s="103"/>
-      <c r="T1" s="103"/>
-      <c r="U1" s="103"/>
-      <c r="V1" s="103"/>
-      <c r="W1" s="103"/>
-      <c r="X1" s="103"/>
-      <c r="Y1" s="103"/>
-      <c r="Z1" s="103"/>
+      <c r="P1" s="96"/>
+      <c r="Q1" s="96"/>
+      <c r="R1" s="96"/>
+      <c r="S1" s="96"/>
+      <c r="T1" s="96"/>
+      <c r="U1" s="96"/>
+      <c r="V1" s="96"/>
+      <c r="W1" s="96"/>
+      <c r="X1" s="96"/>
+      <c r="Y1" s="96"/>
+      <c r="Z1" s="96"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="C2" s="5" t="s">
@@ -42165,7 +43082,7 @@
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A3" s="95" t="s">
+      <c r="A3" s="98" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="10" t="s">
@@ -42247,7 +43164,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A4" s="96"/>
+      <c r="A4" s="99"/>
       <c r="B4" s="11" t="s">
         <v>45</v>
       </c>
@@ -42325,7 +43242,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A5" s="96"/>
+      <c r="A5" s="99"/>
       <c r="B5" s="11" t="s">
         <v>46</v>
       </c>
@@ -42403,7 +43320,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A6" s="96"/>
+      <c r="A6" s="99"/>
       <c r="B6" s="12" t="s">
         <v>47</v>
       </c>
@@ -42481,7 +43398,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A7" s="96"/>
+      <c r="A7" s="99"/>
       <c r="B7" s="10" t="s">
         <v>48</v>
       </c>
@@ -42561,7 +43478,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A8" s="96"/>
+      <c r="A8" s="99"/>
       <c r="B8" s="11" t="s">
         <v>49</v>
       </c>
@@ -42639,7 +43556,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A9" s="96"/>
+      <c r="A9" s="99"/>
       <c r="B9" s="11" t="s">
         <v>50</v>
       </c>
@@ -42717,7 +43634,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A10" s="96"/>
+      <c r="A10" s="99"/>
       <c r="B10" s="12" t="s">
         <v>51</v>
       </c>
@@ -42795,7 +43712,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A11" s="97" t="s">
+      <c r="A11" s="100" t="s">
         <v>58</v>
       </c>
       <c r="B11" s="10" t="s">
@@ -42877,7 +43794,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A12" s="96"/>
+      <c r="A12" s="99"/>
       <c r="B12" s="11" t="s">
         <v>45</v>
       </c>
@@ -42955,7 +43872,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A13" s="96"/>
+      <c r="A13" s="99"/>
       <c r="B13" s="11" t="s">
         <v>46</v>
       </c>
@@ -43033,7 +43950,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A14" s="96"/>
+      <c r="A14" s="99"/>
       <c r="B14" s="12" t="s">
         <v>47</v>
       </c>
@@ -43111,7 +44028,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A15" s="96"/>
+      <c r="A15" s="99"/>
       <c r="B15" s="10" t="s">
         <v>48</v>
       </c>
@@ -43191,7 +44108,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A16" s="96"/>
+      <c r="A16" s="99"/>
       <c r="B16" s="11" t="s">
         <v>49</v>
       </c>
@@ -43268,8 +44185,8 @@
         <v>0.55479309627781204</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A17" s="96"/>
+    <row r="17" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A17" s="99"/>
       <c r="B17" s="11" t="s">
         <v>50</v>
       </c>
@@ -43346,8 +44263,8 @@
         <v>0.66749844042420403</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A18" s="98"/>
+    <row r="18" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A18" s="101"/>
       <c r="B18" s="12" t="s">
         <v>51</v>
       </c>
@@ -43424,24 +44341,77 @@
         <v>0.70534414639218002</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="C24" s="102" t="s">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="AD22" s="105" t="s">
         <v>55</v>
       </c>
-      <c r="D24" s="102"/>
-      <c r="E24" s="102"/>
-      <c r="F24" s="102"/>
-      <c r="G24" s="102"/>
-      <c r="H24" s="102"/>
-      <c r="I24" s="102"/>
-      <c r="J24" s="102"/>
-      <c r="K24" s="102"/>
-      <c r="L24" s="102"/>
-      <c r="M24" s="102"/>
-      <c r="N24" s="102"/>
-      <c r="O24" s="102"/>
+      <c r="AE22" s="105"/>
+      <c r="AF22" s="105"/>
+      <c r="AG22" s="113" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH22" s="114"/>
+      <c r="AI22" s="115"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="AD23" s="95" t="s">
+        <v>91</v>
+      </c>
+      <c r="AE23" s="88" t="s">
+        <v>94</v>
+      </c>
+      <c r="AF23" s="89" t="s">
+        <v>76</v>
+      </c>
+      <c r="AG23" s="88" t="s">
+        <v>91</v>
+      </c>
+      <c r="AH23" s="88" t="s">
+        <v>94</v>
+      </c>
+      <c r="AI23" s="89" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:35" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="105" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" s="105"/>
+      <c r="E24" s="105"/>
+      <c r="F24" s="105"/>
+      <c r="G24" s="105"/>
+      <c r="H24" s="105"/>
+      <c r="I24" s="105"/>
+      <c r="J24" s="105"/>
+      <c r="K24" s="105"/>
+      <c r="L24" s="105"/>
+      <c r="M24" s="105"/>
+      <c r="N24" s="105"/>
+      <c r="O24" s="105"/>
+      <c r="AC24" s="107" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD24" s="116">
+        <v>1.5990698769762201E-4</v>
+      </c>
+      <c r="AE24" s="116">
+        <v>3.85467830722857E-4</v>
+      </c>
+      <c r="AF24" s="116">
+        <v>0.49919999999999998</v>
+      </c>
+      <c r="AG24" s="116">
+        <v>1.24406389982962E-3</v>
+      </c>
+      <c r="AH24" s="116">
+        <v>3.0864644844258902E-3</v>
+      </c>
+      <c r="AI24" s="116">
+        <v>0.49878422443447601</v>
+      </c>
+    </row>
+    <row r="25" spans="1:35" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="C25" s="86" t="s">
         <v>89</v>
       </c>
@@ -43481,8 +44451,29 @@
       <c r="O25" s="89" t="s">
         <v>76</v>
       </c>
+      <c r="AC25" s="111" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD25" s="51">
+        <v>6.1156950869999997E-2</v>
+      </c>
+      <c r="AE25" s="51">
+        <v>3.6881318519999998E-2</v>
+      </c>
+      <c r="AF25" s="59">
+        <v>0.5</v>
+      </c>
+      <c r="AG25" s="51">
+        <v>0.56630378532000003</v>
+      </c>
+      <c r="AH25" s="51">
+        <v>1.1330529172299999</v>
+      </c>
+      <c r="AI25" s="59">
+        <v>0.50609999999999999</v>
+      </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.2">
       <c r="B26" s="90" t="s">
         <v>88</v>
       </c>
@@ -43525,26 +44516,68 @@
       <c r="O26" s="92">
         <v>0.49919999999999998</v>
       </c>
+      <c r="AC26" s="108" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD26" s="48">
+        <v>9.4283246605142298E-2</v>
+      </c>
+      <c r="AE26" s="48">
+        <v>0.19932026734902</v>
+      </c>
+      <c r="AF26" s="57">
+        <v>0.6512</v>
+      </c>
+      <c r="AG26" s="48">
+        <v>0.41905841243000003</v>
+      </c>
+      <c r="AH26" s="48">
+        <v>0.91158193398999998</v>
+      </c>
+      <c r="AI26" s="57">
+        <v>0.59299999999999997</v>
+      </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.2">
       <c r="B27" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C27" s="99"/>
-      <c r="D27" s="100"/>
-      <c r="E27" s="100"/>
-      <c r="F27" s="100"/>
-      <c r="G27" s="100"/>
-      <c r="H27" s="100"/>
-      <c r="I27" s="100"/>
-      <c r="J27" s="100"/>
-      <c r="K27" s="100"/>
-      <c r="L27" s="100"/>
-      <c r="M27" s="100"/>
-      <c r="N27" s="100"/>
-      <c r="O27" s="101"/>
+      <c r="C27" s="102"/>
+      <c r="D27" s="103"/>
+      <c r="E27" s="103"/>
+      <c r="F27" s="103"/>
+      <c r="G27" s="103"/>
+      <c r="H27" s="103"/>
+      <c r="I27" s="103"/>
+      <c r="J27" s="103"/>
+      <c r="K27" s="103"/>
+      <c r="L27" s="103"/>
+      <c r="M27" s="103"/>
+      <c r="N27" s="103"/>
+      <c r="O27" s="104"/>
+      <c r="AC27" s="108" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD27" s="48">
+        <v>8.8007029921725599E-2</v>
+      </c>
+      <c r="AE27" s="48">
+        <v>0.190747163168177</v>
+      </c>
+      <c r="AF27" s="57">
+        <v>0.65049999999999997</v>
+      </c>
+      <c r="AG27" s="48">
+        <v>0.400310795937176</v>
+      </c>
+      <c r="AH27" s="48">
+        <v>0.87728148311072096</v>
+      </c>
+      <c r="AI27" s="57">
+        <v>0.59240000000000004</v>
+      </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.2">
       <c r="B28" s="41" t="s">
         <v>44</v>
       </c>
@@ -43587,8 +44620,29 @@
       <c r="O28" s="56">
         <v>0.5</v>
       </c>
+      <c r="AC28" s="108" t="s">
+        <v>47</v>
+      </c>
+      <c r="AD28" s="48">
+        <v>8.4665653308380995E-2</v>
+      </c>
+      <c r="AE28" s="48">
+        <v>0.18462541982283101</v>
+      </c>
+      <c r="AF28" s="57">
+        <v>0.65</v>
+      </c>
+      <c r="AG28" s="48">
+        <v>0.432913959118917</v>
+      </c>
+      <c r="AH28" s="48">
+        <v>0.93631801659094904</v>
+      </c>
+      <c r="AI28" s="57">
+        <v>0.59409999999999996</v>
+      </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.2">
       <c r="B29" s="43" t="s">
         <v>45</v>
       </c>
@@ -43631,8 +44685,29 @@
       <c r="O29" s="57">
         <v>0.6512</v>
       </c>
+      <c r="AC29" s="117" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD29" s="69">
+        <v>6.8759643120000005E-2</v>
+      </c>
+      <c r="AE29" s="69">
+        <v>4.2822447079999999E-2</v>
+      </c>
+      <c r="AF29" s="70">
+        <v>0.5</v>
+      </c>
+      <c r="AG29" s="69">
+        <v>0.49766462398518801</v>
+      </c>
+      <c r="AH29" s="69">
+        <v>1.1805037383069199</v>
+      </c>
+      <c r="AI29" s="70">
+        <v>0.5585</v>
+      </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.2">
       <c r="B30" s="43" t="s">
         <v>46</v>
       </c>
@@ -43675,8 +44750,29 @@
       <c r="O30" s="57">
         <v>0.65049999999999997</v>
       </c>
+      <c r="AC30" s="108" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD30" s="48">
+        <v>0.13048717966541101</v>
+      </c>
+      <c r="AE30" s="48">
+        <v>0.27160174746214699</v>
+      </c>
+      <c r="AF30" s="57">
+        <v>0.63129999999999997</v>
+      </c>
+      <c r="AG30" s="48">
+        <v>0.49614977318761799</v>
+      </c>
+      <c r="AH30" s="48">
+        <v>1.1083407433981101</v>
+      </c>
+      <c r="AI30" s="57">
+        <v>0.60629999999999995</v>
+      </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.2">
       <c r="B31" s="43" t="s">
         <v>47</v>
       </c>
@@ -43719,8 +44815,29 @@
       <c r="O31" s="57">
         <v>0.65</v>
       </c>
+      <c r="AC31" s="108" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD31" s="48">
+        <v>0.13564035838091101</v>
+      </c>
+      <c r="AE31" s="48">
+        <v>0.28025989021426101</v>
+      </c>
+      <c r="AF31" s="57">
+        <v>0.6331</v>
+      </c>
+      <c r="AG31" s="48">
+        <v>0.47398419904918099</v>
+      </c>
+      <c r="AH31" s="48">
+        <v>1.0442495117400901</v>
+      </c>
+      <c r="AI31" s="57">
+        <v>0.60750000000000004</v>
+      </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:35" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B32" s="66" t="s">
         <v>75</v>
       </c>
@@ -43763,8 +44880,29 @@
       <c r="O32" s="70">
         <v>0.5</v>
       </c>
+      <c r="AC32" s="110" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD32" s="49">
+        <v>0.12772706654272301</v>
+      </c>
+      <c r="AE32" s="49">
+        <v>0.26066474033762499</v>
+      </c>
+      <c r="AF32" s="58">
+        <v>0.63219999999999998</v>
+      </c>
+      <c r="AG32" s="49">
+        <v>0.49742479418236102</v>
+      </c>
+      <c r="AH32" s="49">
+        <v>1.10265551075672</v>
+      </c>
+      <c r="AI32" s="58">
+        <v>0.60640000000000005</v>
+      </c>
     </row>
-    <row r="33" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:35" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B33" s="43" t="s">
         <v>68</v>
       </c>
@@ -43818,21 +44956,29 @@
       <c r="Z33" s="40"/>
       <c r="AA33" s="40"/>
       <c r="AB33" s="40"/>
-      <c r="AC33" s="40"/>
-      <c r="AD33" s="40"/>
-      <c r="AE33" s="40"/>
-      <c r="AF33" s="40"/>
-      <c r="AG33" s="40"/>
-      <c r="AH33" s="40"/>
-      <c r="AI33" s="40"/>
-      <c r="AJ33" s="40"/>
-      <c r="AK33" s="40"/>
-      <c r="AL33" s="40"/>
-      <c r="AM33" s="40"/>
-      <c r="AN33" s="40"/>
-      <c r="AO33" s="40"/>
+      <c r="AC33" s="111" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD33" s="51">
+        <v>5.6908387560000002E-2</v>
+      </c>
+      <c r="AE33" s="51">
+        <v>3.6486215439999997E-2</v>
+      </c>
+      <c r="AF33" s="59">
+        <v>0.5</v>
+      </c>
+      <c r="AG33" s="51">
+        <v>0.22306052859442299</v>
+      </c>
+      <c r="AH33" s="51">
+        <v>0.57247079603464301</v>
+      </c>
+      <c r="AI33" s="59">
+        <v>0.5</v>
+      </c>
     </row>
-    <row r="34" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B34" s="43" t="s">
         <v>69</v>
       </c>
@@ -43886,21 +45032,29 @@
       <c r="Z34" s="40"/>
       <c r="AA34" s="40"/>
       <c r="AB34" s="40"/>
-      <c r="AC34" s="40"/>
-      <c r="AD34" s="40"/>
-      <c r="AE34" s="40"/>
-      <c r="AF34" s="40"/>
-      <c r="AG34" s="40"/>
-      <c r="AH34" s="40"/>
-      <c r="AI34" s="40"/>
-      <c r="AJ34" s="40"/>
-      <c r="AK34" s="40"/>
-      <c r="AL34" s="40"/>
-      <c r="AM34" s="40"/>
-      <c r="AN34" s="40"/>
-      <c r="AO34" s="40"/>
+      <c r="AC34" s="108" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD34" s="48">
+        <v>9.4283246605142298E-2</v>
+      </c>
+      <c r="AE34" s="48">
+        <v>0.19932026734902</v>
+      </c>
+      <c r="AF34" s="57">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="AG34" s="48">
+        <v>0.53968205047320095</v>
+      </c>
+      <c r="AH34" s="48">
+        <v>1.1832514378477199</v>
+      </c>
+      <c r="AI34" s="57">
+        <v>0.63049999999999995</v>
+      </c>
     </row>
-    <row r="35" spans="2:41" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:35" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B35" s="45" t="s">
         <v>70</v>
       </c>
@@ -43954,21 +45108,29 @@
       <c r="Z35" s="40"/>
       <c r="AA35" s="40"/>
       <c r="AB35" s="40"/>
-      <c r="AC35" s="40"/>
-      <c r="AD35" s="40"/>
-      <c r="AE35" s="40"/>
-      <c r="AF35" s="40"/>
-      <c r="AG35" s="40"/>
-      <c r="AH35" s="40"/>
-      <c r="AI35" s="40"/>
-      <c r="AJ35" s="40"/>
-      <c r="AK35" s="40"/>
-      <c r="AL35" s="40"/>
-      <c r="AM35" s="40"/>
-      <c r="AN35" s="40"/>
-      <c r="AO35" s="40"/>
+      <c r="AC35" s="108" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD35" s="48">
+        <v>8.8007029921725599E-2</v>
+      </c>
+      <c r="AE35" s="48">
+        <v>0.190747163168177</v>
+      </c>
+      <c r="AF35" s="57">
+        <v>0.71319999999999995</v>
+      </c>
+      <c r="AG35" s="48">
+        <v>0.45501519469798102</v>
+      </c>
+      <c r="AH35" s="48">
+        <v>1.0246348663465901</v>
+      </c>
+      <c r="AI35" s="57">
+        <v>0.63039999999999996</v>
+      </c>
     </row>
-    <row r="36" spans="2:41" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:35" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B36" s="54" t="s">
         <v>48</v>
       </c>
@@ -44022,21 +45184,29 @@
       <c r="Z36" s="40"/>
       <c r="AA36" s="40"/>
       <c r="AB36" s="40"/>
-      <c r="AC36" s="40"/>
-      <c r="AD36" s="40"/>
-      <c r="AE36" s="40"/>
-      <c r="AF36" s="40"/>
-      <c r="AG36" s="40"/>
-      <c r="AH36" s="40"/>
-      <c r="AI36" s="40"/>
-      <c r="AJ36" s="40"/>
-      <c r="AK36" s="40"/>
-      <c r="AL36" s="40"/>
-      <c r="AM36" s="40"/>
-      <c r="AN36" s="40"/>
-      <c r="AO36" s="40"/>
+      <c r="AC36" s="108" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD36" s="48">
+        <v>0.30389051417097901</v>
+      </c>
+      <c r="AE36" s="48">
+        <v>0.63120965714843202</v>
+      </c>
+      <c r="AF36" s="80">
+        <v>0.71679999999999999</v>
+      </c>
+      <c r="AG36" s="48">
+        <v>0.46698380202338502</v>
+      </c>
+      <c r="AH36" s="48">
+        <v>1.0579946893515</v>
+      </c>
+      <c r="AI36" s="57">
+        <v>0.63129999999999997</v>
+      </c>
     </row>
-    <row r="37" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B37" s="43" t="s">
         <v>49</v>
       </c>
@@ -44079,8 +45249,29 @@
       <c r="O37" s="57">
         <v>0.71499999999999997</v>
       </c>
+      <c r="AC37" s="109" t="s">
+        <v>71</v>
+      </c>
+      <c r="AD37" s="69">
+        <v>6.3393036829999999E-2</v>
+      </c>
+      <c r="AE37" s="69">
+        <v>4.1257850950000001E-2</v>
+      </c>
+      <c r="AF37" s="70">
+        <v>0.5</v>
+      </c>
+      <c r="AG37" s="69">
+        <v>0.20240815556369701</v>
+      </c>
+      <c r="AH37" s="69">
+        <v>0.51803475107129804</v>
+      </c>
+      <c r="AI37" s="70">
+        <v>0.5</v>
+      </c>
     </row>
-    <row r="38" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B38" s="43" t="s">
         <v>50</v>
       </c>
@@ -44123,8 +45314,29 @@
       <c r="O38" s="57">
         <v>0.71319999999999995</v>
       </c>
+      <c r="AC38" s="108" t="s">
+        <v>72</v>
+      </c>
+      <c r="AD38" s="48">
+        <v>0.28173425680133901</v>
+      </c>
+      <c r="AE38" s="48">
+        <v>0.58945529813573005</v>
+      </c>
+      <c r="AF38" s="57">
+        <v>0.71230000000000004</v>
+      </c>
+      <c r="AG38" s="48">
+        <v>0.47297421949302298</v>
+      </c>
+      <c r="AH38" s="48">
+        <v>1.0370412173102901</v>
+      </c>
+      <c r="AI38" s="57">
+        <v>0.62619999999999998</v>
+      </c>
     </row>
-    <row r="39" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B39" s="43" t="s">
         <v>51</v>
       </c>
@@ -44167,8 +45379,29 @@
       <c r="O39" s="80">
         <v>0.71679999999999999</v>
       </c>
+      <c r="AC39" s="108" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD39" s="48">
+        <v>0.30598852213529798</v>
+      </c>
+      <c r="AE39" s="48">
+        <v>0.62053947586219205</v>
+      </c>
+      <c r="AF39" s="57">
+        <v>0.7077</v>
+      </c>
+      <c r="AG39" s="48">
+        <v>0.52561685564685801</v>
+      </c>
+      <c r="AH39" s="48">
+        <v>1.1852013775805299</v>
+      </c>
+      <c r="AI39" s="57">
+        <v>0.63380000000000003</v>
+      </c>
     </row>
-    <row r="40" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B40" s="66" t="s">
         <v>71</v>
       </c>
@@ -44211,8 +45444,29 @@
       <c r="O40" s="70">
         <v>0.5</v>
       </c>
+      <c r="AC40" s="112" t="s">
+        <v>74</v>
+      </c>
+      <c r="AD40" s="73">
+        <v>0.30939914773180999</v>
+      </c>
+      <c r="AE40" s="73">
+        <v>0.65151138345691895</v>
+      </c>
+      <c r="AF40" s="60">
+        <v>0.70899999999999996</v>
+      </c>
+      <c r="AG40" s="73">
+        <v>0.57279847152926999</v>
+      </c>
+      <c r="AH40" s="73">
+        <v>1.26618403019026</v>
+      </c>
+      <c r="AI40" s="79">
+        <v>0.64700000000000002</v>
+      </c>
     </row>
-    <row r="41" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B41" s="43" t="s">
         <v>72</v>
       </c>
@@ -44256,7 +45510,7 @@
         <v>0.71230000000000004</v>
       </c>
     </row>
-    <row r="42" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B42" s="43" t="s">
         <v>73</v>
       </c>
@@ -44300,7 +45554,7 @@
         <v>0.7077</v>
       </c>
     </row>
-    <row r="43" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B43" s="55" t="s">
         <v>74</v>
       </c>
@@ -44344,24 +45598,24 @@
         <v>0.70899999999999996</v>
       </c>
     </row>
-    <row r="45" spans="2:41" x14ac:dyDescent="0.2">
-      <c r="C45" s="102" t="s">
+    <row r="45" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="C45" s="105" t="s">
         <v>56</v>
       </c>
-      <c r="D45" s="102"/>
-      <c r="E45" s="102"/>
-      <c r="F45" s="102"/>
-      <c r="G45" s="102"/>
-      <c r="H45" s="102"/>
-      <c r="I45" s="102"/>
-      <c r="J45" s="102"/>
-      <c r="K45" s="102"/>
-      <c r="L45" s="102"/>
-      <c r="M45" s="102"/>
-      <c r="N45" s="102"/>
-      <c r="O45" s="102"/>
+      <c r="D45" s="105"/>
+      <c r="E45" s="105"/>
+      <c r="F45" s="105"/>
+      <c r="G45" s="105"/>
+      <c r="H45" s="105"/>
+      <c r="I45" s="105"/>
+      <c r="J45" s="105"/>
+      <c r="K45" s="105"/>
+      <c r="L45" s="105"/>
+      <c r="M45" s="105"/>
+      <c r="N45" s="105"/>
+      <c r="O45" s="105"/>
     </row>
-    <row r="46" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:35" x14ac:dyDescent="0.2">
       <c r="C46" s="86" t="s">
         <v>89</v>
       </c>
@@ -44402,7 +45656,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="47" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B47" s="91" t="s">
         <v>88</v>
       </c>
@@ -44446,23 +45700,23 @@
         <v>0.49878422443447601</v>
       </c>
     </row>
-    <row r="48" spans="2:41" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B48" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C48" s="99"/>
-      <c r="D48" s="100"/>
-      <c r="E48" s="100"/>
-      <c r="F48" s="100"/>
-      <c r="G48" s="100"/>
-      <c r="H48" s="100"/>
-      <c r="I48" s="100"/>
-      <c r="J48" s="100"/>
-      <c r="K48" s="100"/>
-      <c r="L48" s="100"/>
-      <c r="M48" s="100"/>
-      <c r="N48" s="100"/>
-      <c r="O48" s="101"/>
+      <c r="C48" s="102"/>
+      <c r="D48" s="103"/>
+      <c r="E48" s="103"/>
+      <c r="F48" s="103"/>
+      <c r="G48" s="103"/>
+      <c r="H48" s="103"/>
+      <c r="I48" s="103"/>
+      <c r="J48" s="103"/>
+      <c r="K48" s="103"/>
+      <c r="L48" s="103"/>
+      <c r="M48" s="103"/>
+      <c r="N48" s="103"/>
+      <c r="O48" s="104"/>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B49" s="41" t="s">
@@ -44641,8 +45895,8 @@
       </c>
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B53" s="66" t="s">
-        <v>75</v>
+      <c r="B53" s="118" t="s">
+        <v>67</v>
       </c>
       <c r="C53" s="67">
         <v>0.248668171781085</v>
@@ -45169,18 +46423,20 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
+    <mergeCell ref="AD22:AF22"/>
+    <mergeCell ref="AG22:AI22"/>
+    <mergeCell ref="C48:O48"/>
+    <mergeCell ref="C45:O45"/>
+    <mergeCell ref="C24:O24"/>
     <mergeCell ref="C1:N1"/>
     <mergeCell ref="O1:Z1"/>
     <mergeCell ref="A3:A10"/>
     <mergeCell ref="A11:A18"/>
     <mergeCell ref="C27:O27"/>
-    <mergeCell ref="C48:O48"/>
-    <mergeCell ref="C45:O45"/>
-    <mergeCell ref="C24:O24"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:C18">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -45188,7 +46444,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="107">
+    <cfRule type="colorScale" priority="136">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -45200,7 +46456,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D18">
-    <cfRule type="colorScale" priority="105">
+    <cfRule type="colorScale" priority="134">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -45210,7 +46466,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E18">
-    <cfRule type="colorScale" priority="104">
+    <cfRule type="colorScale" priority="133">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -45220,7 +46476,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:F18">
-    <cfRule type="colorScale" priority="103">
+    <cfRule type="colorScale" priority="132">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -45230,7 +46486,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G18">
-    <cfRule type="colorScale" priority="102">
+    <cfRule type="colorScale" priority="131">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -45240,7 +46496,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H18">
-    <cfRule type="colorScale" priority="101">
+    <cfRule type="colorScale" priority="130">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -45250,7 +46506,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:I18">
-    <cfRule type="colorScale" priority="100">
+    <cfRule type="colorScale" priority="129">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -45260,6 +46516,176 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J18">
+    <cfRule type="colorScale" priority="128">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3:K18">
+    <cfRule type="colorScale" priority="127">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L3:L18">
+    <cfRule type="colorScale" priority="126">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3:M18">
+    <cfRule type="colorScale" priority="125">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N3:N18">
+    <cfRule type="colorScale" priority="124">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O3:O18">
+    <cfRule type="colorScale" priority="123">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P3:P18">
+    <cfRule type="colorScale" priority="122">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q3:Q18">
+    <cfRule type="colorScale" priority="121">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R3:R18">
+    <cfRule type="colorScale" priority="120">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S3:S18">
+    <cfRule type="colorScale" priority="119">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T3:T18">
+    <cfRule type="colorScale" priority="118">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U3:U18">
+    <cfRule type="colorScale" priority="117">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V3:V18">
+    <cfRule type="colorScale" priority="116">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W3:W18">
+    <cfRule type="colorScale" priority="115">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X3:X18">
+    <cfRule type="colorScale" priority="114">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y3:Y18">
+    <cfRule type="colorScale" priority="113">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z3:Z18">
+    <cfRule type="colorScale" priority="112">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O28:O43">
     <cfRule type="colorScale" priority="99">
       <colorScale>
         <cfvo type="min"/>
@@ -45269,8 +46695,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K18">
-    <cfRule type="colorScale" priority="98">
+  <conditionalFormatting sqref="L28:L43">
+    <cfRule type="colorScale" priority="76">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -45279,8 +46705,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L3:L18">
-    <cfRule type="colorScale" priority="97">
+  <conditionalFormatting sqref="M28:M43">
+    <cfRule type="colorScale" priority="75">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -45289,8 +46715,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M18">
-    <cfRule type="colorScale" priority="96">
+  <conditionalFormatting sqref="N28:N43">
+    <cfRule type="colorScale" priority="74">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -45299,8 +46725,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3:N18">
-    <cfRule type="colorScale" priority="95">
+  <conditionalFormatting sqref="C28:C43">
+    <cfRule type="colorScale" priority="73">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -45309,8 +46735,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O3:O18">
-    <cfRule type="colorScale" priority="94">
+  <conditionalFormatting sqref="D28:D43">
+    <cfRule type="colorScale" priority="72">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -45319,8 +46745,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P18">
-    <cfRule type="colorScale" priority="93">
+  <conditionalFormatting sqref="E28:E43">
+    <cfRule type="colorScale" priority="71">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -45329,107 +46755,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q3:Q18">
-    <cfRule type="colorScale" priority="92">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R3:R18">
-    <cfRule type="colorScale" priority="91">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S3:S18">
-    <cfRule type="colorScale" priority="90">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T3:T18">
-    <cfRule type="colorScale" priority="89">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="U3:U18">
-    <cfRule type="colorScale" priority="88">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V3:V18">
-    <cfRule type="colorScale" priority="87">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="W3:W18">
-    <cfRule type="colorScale" priority="86">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X3:X18">
-    <cfRule type="colorScale" priority="85">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y3:Y18">
-    <cfRule type="colorScale" priority="84">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Z3:Z18">
-    <cfRule type="colorScale" priority="83">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O28:O43">
+  <conditionalFormatting sqref="F28:F43">
     <cfRule type="colorScale" priority="70">
       <colorScale>
         <cfvo type="min"/>
@@ -45439,8 +46765,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L28:L43">
-    <cfRule type="colorScale" priority="47">
+  <conditionalFormatting sqref="G28:G43">
+    <cfRule type="colorScale" priority="69">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -45449,8 +46775,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M28:M43">
-    <cfRule type="colorScale" priority="46">
+  <conditionalFormatting sqref="H28:H43">
+    <cfRule type="colorScale" priority="68">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -45459,8 +46785,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N28:N43">
-    <cfRule type="colorScale" priority="45">
+  <conditionalFormatting sqref="I28:I43">
+    <cfRule type="colorScale" priority="67">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -45469,8 +46795,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C28:C43">
-    <cfRule type="colorScale" priority="44">
+  <conditionalFormatting sqref="J28:J43">
+    <cfRule type="colorScale" priority="66">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -45479,7 +46805,17 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D28:D43">
+  <conditionalFormatting sqref="K28:K43">
+    <cfRule type="colorScale" priority="65">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O49:O64">
     <cfRule type="colorScale" priority="43">
       <colorScale>
         <cfvo type="min"/>
@@ -45489,7 +46825,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E28:E43">
+  <conditionalFormatting sqref="L49:L64">
     <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="min"/>
@@ -45499,7 +46835,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F28:F43">
+  <conditionalFormatting sqref="M49:M64">
     <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="min"/>
@@ -45509,7 +46845,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G28:G43">
+  <conditionalFormatting sqref="N49:N64">
     <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="min"/>
@@ -45519,7 +46855,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H28:H43">
+  <conditionalFormatting sqref="C49:C64">
     <cfRule type="colorScale" priority="39">
       <colorScale>
         <cfvo type="min"/>
@@ -45529,7 +46865,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I28:I43">
+  <conditionalFormatting sqref="D49:D64">
     <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="min"/>
@@ -45539,7 +46875,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J28:J43">
+  <conditionalFormatting sqref="E49:E64">
     <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="min"/>
@@ -45549,7 +46885,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K28:K43">
+  <conditionalFormatting sqref="F49:F64">
     <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="min"/>
@@ -45559,88 +46895,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O49:O64">
-    <cfRule type="colorScale" priority="14">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L49:L64">
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M49:M64">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N49:N64">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C64">
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D49:D64">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E49:E64">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F49:F64">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="G49:G64">
-    <cfRule type="colorScale" priority="6">
+    <cfRule type="colorScale" priority="35">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -45650,7 +46906,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H49:H64">
-    <cfRule type="colorScale" priority="5">
+    <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -45660,7 +46916,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I49:I64">
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="33">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -45670,6 +46926,56 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J49:J64">
+    <cfRule type="colorScale" priority="32">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K49:K64">
+    <cfRule type="colorScale" priority="31">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF25:AF40">
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD25:AD40">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE25:AE40">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI25:AI40">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -45679,8 +46985,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K49:K64">
+  <conditionalFormatting sqref="AG25:AG40">
     <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH25:AH40">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -45699,7 +47015,7 @@
   <dimension ref="A1:R46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D39" sqref="D39:D46"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -45724,38 +47040,38 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="29"/>
-      <c r="B1" s="105" t="s">
+      <c r="B1" s="106" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="105"/>
-      <c r="D1" s="105" t="s">
+      <c r="C1" s="106"/>
+      <c r="D1" s="106" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="105"/>
-      <c r="F1" s="105" t="s">
+      <c r="E1" s="106"/>
+      <c r="F1" s="106" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="105"/>
-      <c r="H1" s="105" t="s">
+      <c r="G1" s="106"/>
+      <c r="H1" s="106" t="s">
         <v>60</v>
       </c>
-      <c r="I1" s="105"/>
-      <c r="J1" s="105" t="s">
+      <c r="I1" s="106"/>
+      <c r="J1" s="106" t="s">
         <v>61</v>
       </c>
-      <c r="K1" s="105"/>
-      <c r="L1" s="105" t="s">
+      <c r="K1" s="106"/>
+      <c r="L1" s="106" t="s">
         <v>49</v>
       </c>
-      <c r="M1" s="105"/>
-      <c r="N1" s="105" t="s">
+      <c r="M1" s="106"/>
+      <c r="N1" s="106" t="s">
         <v>50</v>
       </c>
-      <c r="O1" s="105"/>
-      <c r="P1" s="105" t="s">
+      <c r="O1" s="106"/>
+      <c r="P1" s="106" t="s">
         <v>51</v>
       </c>
-      <c r="Q1" s="105"/>
+      <c r="Q1" s="106"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="29"/>
@@ -45926,7 +47242,7 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A11" s="95" t="s">
+      <c r="A11" s="98" t="s">
         <v>57</v>
       </c>
       <c r="B11" s="10" t="s">
@@ -45941,7 +47257,7 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A12" s="96"/>
+      <c r="A12" s="99"/>
       <c r="B12" s="11" t="s">
         <v>45</v>
       </c>
@@ -45965,7 +47281,7 @@
       <c r="Q12" s="39"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A13" s="96"/>
+      <c r="A13" s="99"/>
       <c r="B13" s="11" t="s">
         <v>46</v>
       </c>
@@ -45989,7 +47305,7 @@
       <c r="Q13" s="39"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A14" s="96"/>
+      <c r="A14" s="99"/>
       <c r="B14" s="12" t="s">
         <v>47</v>
       </c>
@@ -46013,7 +47329,7 @@
       <c r="Q14" s="39"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A15" s="96"/>
+      <c r="A15" s="99"/>
       <c r="B15" s="10" t="s">
         <v>48</v>
       </c>
@@ -46037,7 +47353,7 @@
       <c r="Q15" s="39"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A16" s="96"/>
+      <c r="A16" s="99"/>
       <c r="B16" s="11" t="s">
         <v>49</v>
       </c>
@@ -46061,7 +47377,7 @@
       <c r="Q16" s="39"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A17" s="96"/>
+      <c r="A17" s="99"/>
       <c r="B17" s="11" t="s">
         <v>50</v>
       </c>
@@ -46085,7 +47401,7 @@
       <c r="Q17" s="39"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A18" s="96"/>
+      <c r="A18" s="99"/>
       <c r="B18" s="12" t="s">
         <v>51</v>
       </c>
@@ -46109,7 +47425,7 @@
       <c r="Q18" s="39"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A19" s="97" t="s">
+      <c r="A19" s="100" t="s">
         <v>58</v>
       </c>
       <c r="B19" s="10" t="s">
@@ -46135,7 +47451,7 @@
       <c r="Q19" s="39"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A20" s="96"/>
+      <c r="A20" s="99"/>
       <c r="B20" s="11" t="s">
         <v>68</v>
       </c>
@@ -46159,7 +47475,7 @@
       <c r="Q20" s="39"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A21" s="96"/>
+      <c r="A21" s="99"/>
       <c r="B21" s="11" t="s">
         <v>69</v>
       </c>
@@ -46183,7 +47499,7 @@
       <c r="Q21" s="39"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A22" s="96"/>
+      <c r="A22" s="99"/>
       <c r="B22" s="12" t="s">
         <v>70</v>
       </c>
@@ -46207,7 +47523,7 @@
       <c r="Q22" s="39"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A23" s="96"/>
+      <c r="A23" s="99"/>
       <c r="B23" s="10" t="s">
         <v>71</v>
       </c>
@@ -46231,7 +47547,7 @@
       <c r="Q23" s="39"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A24" s="96"/>
+      <c r="A24" s="99"/>
       <c r="B24" s="11" t="s">
         <v>72</v>
       </c>
@@ -46255,7 +47571,7 @@
       <c r="Q24" s="39"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A25" s="96"/>
+      <c r="A25" s="99"/>
       <c r="B25" s="11" t="s">
         <v>73</v>
       </c>
@@ -46279,7 +47595,7 @@
       <c r="Q25" s="39"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A26" s="98"/>
+      <c r="A26" s="101"/>
       <c r="B26" s="12" t="s">
         <v>74</v>
       </c>
@@ -46604,16 +47920,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A19:A26"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="L1:M1"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="A11:A18"/>
-    <mergeCell ref="A19:A26"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="C11:C26">
     <cfRule type="colorScale" priority="2">
@@ -50598,8 +51914,8 @@
   </sheetPr>
   <dimension ref="A1:S128"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
list of input models and datasets in the arguements
</commit_message>
<xml_diff>
--- a/output/results_dblp_imdb_fnn_bnn_emb_nns.xlsx
+++ b/output/results_dblp_imdb_fnn_bnn_emb_nns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Github\Fani-Lab\neural_team_formation\dblp\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{137FC677-6B9D-4772-A34A-60EFC91DCB81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{671DD4E8-6710-43F4-8291-420D8E9B732E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -378,7 +378,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -413,6 +413,19 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -742,7 +755,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -915,9 +928,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -948,26 +958,71 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -42954,8 +43009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE483F02-EABB-410C-B581-D071545F3EF7}">
   <dimension ref="A1:AI64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" topLeftCell="H10" workbookViewId="0">
+      <selection activeCell="AC22" sqref="AC22:AI40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -42978,34 +43033,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="C1" s="96" t="s">
+      <c r="C1" s="95" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
-      <c r="L1" s="96"/>
-      <c r="M1" s="96"/>
-      <c r="N1" s="97"/>
-      <c r="O1" s="96" t="s">
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="95"/>
+      <c r="I1" s="95"/>
+      <c r="J1" s="95"/>
+      <c r="K1" s="95"/>
+      <c r="L1" s="95"/>
+      <c r="M1" s="95"/>
+      <c r="N1" s="96"/>
+      <c r="O1" s="95" t="s">
         <v>56</v>
       </c>
-      <c r="P1" s="96"/>
-      <c r="Q1" s="96"/>
-      <c r="R1" s="96"/>
-      <c r="S1" s="96"/>
-      <c r="T1" s="96"/>
-      <c r="U1" s="96"/>
-      <c r="V1" s="96"/>
-      <c r="W1" s="96"/>
-      <c r="X1" s="96"/>
-      <c r="Y1" s="96"/>
-      <c r="Z1" s="96"/>
+      <c r="P1" s="95"/>
+      <c r="Q1" s="95"/>
+      <c r="R1" s="95"/>
+      <c r="S1" s="95"/>
+      <c r="T1" s="95"/>
+      <c r="U1" s="95"/>
+      <c r="V1" s="95"/>
+      <c r="W1" s="95"/>
+      <c r="X1" s="95"/>
+      <c r="Y1" s="95"/>
+      <c r="Z1" s="95"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="C2" s="5" t="s">
@@ -43082,7 +43137,7 @@
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A3" s="98" t="s">
+      <c r="A3" s="97" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="10" t="s">
@@ -43164,7 +43219,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A4" s="99"/>
+      <c r="A4" s="98"/>
       <c r="B4" s="11" t="s">
         <v>45</v>
       </c>
@@ -43242,7 +43297,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A5" s="99"/>
+      <c r="A5" s="98"/>
       <c r="B5" s="11" t="s">
         <v>46</v>
       </c>
@@ -43320,7 +43375,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A6" s="99"/>
+      <c r="A6" s="98"/>
       <c r="B6" s="12" t="s">
         <v>47</v>
       </c>
@@ -43398,7 +43453,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A7" s="99"/>
+      <c r="A7" s="98"/>
       <c r="B7" s="10" t="s">
         <v>48</v>
       </c>
@@ -43478,7 +43533,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A8" s="99"/>
+      <c r="A8" s="98"/>
       <c r="B8" s="11" t="s">
         <v>49</v>
       </c>
@@ -43556,7 +43611,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A9" s="99"/>
+      <c r="A9" s="98"/>
       <c r="B9" s="11" t="s">
         <v>50</v>
       </c>
@@ -43634,7 +43689,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A10" s="99"/>
+      <c r="A10" s="98"/>
       <c r="B10" s="12" t="s">
         <v>51</v>
       </c>
@@ -43712,7 +43767,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A11" s="100" t="s">
+      <c r="A11" s="99" t="s">
         <v>58</v>
       </c>
       <c r="B11" s="10" t="s">
@@ -43794,7 +43849,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A12" s="99"/>
+      <c r="A12" s="98"/>
       <c r="B12" s="11" t="s">
         <v>45</v>
       </c>
@@ -43872,7 +43927,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A13" s="99"/>
+      <c r="A13" s="98"/>
       <c r="B13" s="11" t="s">
         <v>46</v>
       </c>
@@ -43950,7 +44005,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A14" s="99"/>
+      <c r="A14" s="98"/>
       <c r="B14" s="12" t="s">
         <v>47</v>
       </c>
@@ -44028,7 +44083,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A15" s="99"/>
+      <c r="A15" s="98"/>
       <c r="B15" s="10" t="s">
         <v>48</v>
       </c>
@@ -44108,7 +44163,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A16" s="99"/>
+      <c r="A16" s="98"/>
       <c r="B16" s="11" t="s">
         <v>49</v>
       </c>
@@ -44186,7 +44241,7 @@
       </c>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A17" s="99"/>
+      <c r="A17" s="98"/>
       <c r="B17" s="11" t="s">
         <v>50</v>
       </c>
@@ -44264,7 +44319,7 @@
       </c>
     </row>
     <row r="18" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A18" s="101"/>
+      <c r="A18" s="100"/>
       <c r="B18" s="12" t="s">
         <v>51</v>
       </c>
@@ -44342,72 +44397,74 @@
       </c>
     </row>
     <row r="22" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="AD22" s="105" t="s">
+      <c r="AC22" s="107"/>
+      <c r="AD22" s="108" t="s">
         <v>55</v>
       </c>
-      <c r="AE22" s="105"/>
-      <c r="AF22" s="105"/>
-      <c r="AG22" s="113" t="s">
+      <c r="AE22" s="108"/>
+      <c r="AF22" s="108"/>
+      <c r="AG22" s="109" t="s">
         <v>56</v>
       </c>
-      <c r="AH22" s="114"/>
-      <c r="AI22" s="115"/>
+      <c r="AH22" s="110"/>
+      <c r="AI22" s="111"/>
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="AD23" s="95" t="s">
+      <c r="AC23" s="107"/>
+      <c r="AD23" s="112" t="s">
         <v>91</v>
       </c>
-      <c r="AE23" s="88" t="s">
+      <c r="AE23" s="113" t="s">
         <v>94</v>
       </c>
-      <c r="AF23" s="89" t="s">
+      <c r="AF23" s="113" t="s">
         <v>76</v>
       </c>
-      <c r="AG23" s="88" t="s">
+      <c r="AG23" s="113" t="s">
         <v>91</v>
       </c>
-      <c r="AH23" s="88" t="s">
+      <c r="AH23" s="113" t="s">
         <v>94</v>
       </c>
-      <c r="AI23" s="89" t="s">
+      <c r="AI23" s="113" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:35" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="105" t="s">
+      <c r="C24" s="104" t="s">
         <v>55</v>
       </c>
-      <c r="D24" s="105"/>
-      <c r="E24" s="105"/>
-      <c r="F24" s="105"/>
-      <c r="G24" s="105"/>
-      <c r="H24" s="105"/>
-      <c r="I24" s="105"/>
-      <c r="J24" s="105"/>
-      <c r="K24" s="105"/>
-      <c r="L24" s="105"/>
-      <c r="M24" s="105"/>
-      <c r="N24" s="105"/>
-      <c r="O24" s="105"/>
-      <c r="AC24" s="107" t="s">
+      <c r="D24" s="104"/>
+      <c r="E24" s="104"/>
+      <c r="F24" s="104"/>
+      <c r="G24" s="104"/>
+      <c r="H24" s="104"/>
+      <c r="I24" s="104"/>
+      <c r="J24" s="104"/>
+      <c r="K24" s="104"/>
+      <c r="L24" s="104"/>
+      <c r="M24" s="104"/>
+      <c r="N24" s="104"/>
+      <c r="O24" s="104"/>
+      <c r="AC24" s="114" t="s">
         <v>88</v>
       </c>
-      <c r="AD24" s="116">
+      <c r="AD24" s="115">
         <v>1.5990698769762201E-4</v>
       </c>
-      <c r="AE24" s="116">
+      <c r="AE24" s="115">
         <v>3.85467830722857E-4</v>
       </c>
-      <c r="AF24" s="116">
+      <c r="AF24" s="115">
         <v>0.49919999999999998</v>
       </c>
-      <c r="AG24" s="116">
+      <c r="AG24" s="115">
         <v>1.24406389982962E-3</v>
       </c>
-      <c r="AH24" s="116">
+      <c r="AH24" s="115">
         <v>3.0864644844258902E-3</v>
       </c>
-      <c r="AI24" s="116">
+      <c r="AI24" s="115">
         <v>0.49878422443447601</v>
       </c>
     </row>
@@ -44451,25 +44508,25 @@
       <c r="O25" s="89" t="s">
         <v>76</v>
       </c>
-      <c r="AC25" s="111" t="s">
+      <c r="AC25" s="116" t="s">
         <v>44</v>
       </c>
-      <c r="AD25" s="51">
+      <c r="AD25" s="117">
         <v>6.1156950869999997E-2</v>
       </c>
-      <c r="AE25" s="51">
+      <c r="AE25" s="117">
         <v>3.6881318519999998E-2</v>
       </c>
-      <c r="AF25" s="59">
+      <c r="AF25" s="118">
         <v>0.5</v>
       </c>
-      <c r="AG25" s="51">
+      <c r="AG25" s="117">
         <v>0.56630378532000003</v>
       </c>
-      <c r="AH25" s="51">
+      <c r="AH25" s="117">
         <v>1.1330529172299999</v>
       </c>
-      <c r="AI25" s="59">
+      <c r="AI25" s="118">
         <v>0.50609999999999999</v>
       </c>
     </row>
@@ -44516,25 +44573,25 @@
       <c r="O26" s="92">
         <v>0.49919999999999998</v>
       </c>
-      <c r="AC26" s="108" t="s">
+      <c r="AC26" s="119" t="s">
         <v>45</v>
       </c>
-      <c r="AD26" s="48">
+      <c r="AD26" s="120">
         <v>9.4283246605142298E-2</v>
       </c>
-      <c r="AE26" s="48">
+      <c r="AE26" s="120">
         <v>0.19932026734902</v>
       </c>
-      <c r="AF26" s="57">
+      <c r="AF26" s="121">
         <v>0.6512</v>
       </c>
-      <c r="AG26" s="48">
+      <c r="AG26" s="120">
         <v>0.41905841243000003</v>
       </c>
-      <c r="AH26" s="48">
+      <c r="AH26" s="120">
         <v>0.91158193398999998</v>
       </c>
-      <c r="AI26" s="57">
+      <c r="AI26" s="121">
         <v>0.59299999999999997</v>
       </c>
     </row>
@@ -44542,38 +44599,38 @@
       <c r="B27" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C27" s="102"/>
-      <c r="D27" s="103"/>
-      <c r="E27" s="103"/>
-      <c r="F27" s="103"/>
-      <c r="G27" s="103"/>
-      <c r="H27" s="103"/>
-      <c r="I27" s="103"/>
-      <c r="J27" s="103"/>
-      <c r="K27" s="103"/>
-      <c r="L27" s="103"/>
-      <c r="M27" s="103"/>
-      <c r="N27" s="103"/>
-      <c r="O27" s="104"/>
-      <c r="AC27" s="108" t="s">
+      <c r="C27" s="101"/>
+      <c r="D27" s="102"/>
+      <c r="E27" s="102"/>
+      <c r="F27" s="102"/>
+      <c r="G27" s="102"/>
+      <c r="H27" s="102"/>
+      <c r="I27" s="102"/>
+      <c r="J27" s="102"/>
+      <c r="K27" s="102"/>
+      <c r="L27" s="102"/>
+      <c r="M27" s="102"/>
+      <c r="N27" s="102"/>
+      <c r="O27" s="103"/>
+      <c r="AC27" s="119" t="s">
         <v>46</v>
       </c>
-      <c r="AD27" s="48">
+      <c r="AD27" s="120">
         <v>8.8007029921725599E-2</v>
       </c>
-      <c r="AE27" s="48">
+      <c r="AE27" s="120">
         <v>0.190747163168177</v>
       </c>
-      <c r="AF27" s="57">
+      <c r="AF27" s="121">
         <v>0.65049999999999997</v>
       </c>
-      <c r="AG27" s="48">
+      <c r="AG27" s="120">
         <v>0.400310795937176</v>
       </c>
-      <c r="AH27" s="48">
+      <c r="AH27" s="120">
         <v>0.87728148311072096</v>
       </c>
-      <c r="AI27" s="57">
+      <c r="AI27" s="121">
         <v>0.59240000000000004</v>
       </c>
     </row>
@@ -44620,25 +44677,25 @@
       <c r="O28" s="56">
         <v>0.5</v>
       </c>
-      <c r="AC28" s="108" t="s">
+      <c r="AC28" s="119" t="s">
         <v>47</v>
       </c>
-      <c r="AD28" s="48">
+      <c r="AD28" s="120">
         <v>8.4665653308380995E-2</v>
       </c>
-      <c r="AE28" s="48">
+      <c r="AE28" s="120">
         <v>0.18462541982283101</v>
       </c>
-      <c r="AF28" s="57">
+      <c r="AF28" s="121">
         <v>0.65</v>
       </c>
-      <c r="AG28" s="48">
+      <c r="AG28" s="120">
         <v>0.432913959118917</v>
       </c>
-      <c r="AH28" s="48">
+      <c r="AH28" s="120">
         <v>0.93631801659094904</v>
       </c>
-      <c r="AI28" s="57">
+      <c r="AI28" s="121">
         <v>0.59409999999999996</v>
       </c>
     </row>
@@ -44685,25 +44742,25 @@
       <c r="O29" s="57">
         <v>0.6512</v>
       </c>
-      <c r="AC29" s="117" t="s">
+      <c r="AC29" s="122" t="s">
         <v>67</v>
       </c>
-      <c r="AD29" s="69">
+      <c r="AD29" s="123">
         <v>6.8759643120000005E-2</v>
       </c>
-      <c r="AE29" s="69">
+      <c r="AE29" s="123">
         <v>4.2822447079999999E-2</v>
       </c>
-      <c r="AF29" s="70">
+      <c r="AF29" s="124">
         <v>0.5</v>
       </c>
-      <c r="AG29" s="69">
+      <c r="AG29" s="123">
         <v>0.49766462398518801</v>
       </c>
-      <c r="AH29" s="69">
+      <c r="AH29" s="123">
         <v>1.1805037383069199</v>
       </c>
-      <c r="AI29" s="70">
+      <c r="AI29" s="124">
         <v>0.5585</v>
       </c>
     </row>
@@ -44750,25 +44807,25 @@
       <c r="O30" s="57">
         <v>0.65049999999999997</v>
       </c>
-      <c r="AC30" s="108" t="s">
+      <c r="AC30" s="119" t="s">
         <v>68</v>
       </c>
-      <c r="AD30" s="48">
+      <c r="AD30" s="120">
         <v>0.13048717966541101</v>
       </c>
-      <c r="AE30" s="48">
+      <c r="AE30" s="120">
         <v>0.27160174746214699</v>
       </c>
-      <c r="AF30" s="57">
+      <c r="AF30" s="121">
         <v>0.63129999999999997</v>
       </c>
-      <c r="AG30" s="48">
+      <c r="AG30" s="120">
         <v>0.49614977318761799</v>
       </c>
-      <c r="AH30" s="48">
+      <c r="AH30" s="120">
         <v>1.1083407433981101</v>
       </c>
-      <c r="AI30" s="57">
+      <c r="AI30" s="121">
         <v>0.60629999999999995</v>
       </c>
     </row>
@@ -44815,25 +44872,25 @@
       <c r="O31" s="57">
         <v>0.65</v>
       </c>
-      <c r="AC31" s="108" t="s">
+      <c r="AC31" s="119" t="s">
         <v>69</v>
       </c>
-      <c r="AD31" s="48">
+      <c r="AD31" s="120">
         <v>0.13564035838091101</v>
       </c>
-      <c r="AE31" s="48">
+      <c r="AE31" s="120">
         <v>0.28025989021426101</v>
       </c>
-      <c r="AF31" s="57">
+      <c r="AF31" s="121">
         <v>0.6331</v>
       </c>
-      <c r="AG31" s="48">
+      <c r="AG31" s="120">
         <v>0.47398419904918099</v>
       </c>
-      <c r="AH31" s="48">
+      <c r="AH31" s="120">
         <v>1.0442495117400901</v>
       </c>
-      <c r="AI31" s="57">
+      <c r="AI31" s="121">
         <v>0.60750000000000004</v>
       </c>
     </row>
@@ -44880,25 +44937,25 @@
       <c r="O32" s="70">
         <v>0.5</v>
       </c>
-      <c r="AC32" s="110" t="s">
+      <c r="AC32" s="125" t="s">
         <v>70</v>
       </c>
-      <c r="AD32" s="49">
+      <c r="AD32" s="126">
         <v>0.12772706654272301</v>
       </c>
-      <c r="AE32" s="49">
+      <c r="AE32" s="126">
         <v>0.26066474033762499</v>
       </c>
-      <c r="AF32" s="58">
+      <c r="AF32" s="127">
         <v>0.63219999999999998</v>
       </c>
-      <c r="AG32" s="49">
+      <c r="AG32" s="126">
         <v>0.49742479418236102</v>
       </c>
-      <c r="AH32" s="49">
+      <c r="AH32" s="126">
         <v>1.10265551075672</v>
       </c>
-      <c r="AI32" s="58">
+      <c r="AI32" s="127">
         <v>0.60640000000000005</v>
       </c>
     </row>
@@ -44956,25 +45013,25 @@
       <c r="Z33" s="40"/>
       <c r="AA33" s="40"/>
       <c r="AB33" s="40"/>
-      <c r="AC33" s="111" t="s">
+      <c r="AC33" s="116" t="s">
         <v>48</v>
       </c>
-      <c r="AD33" s="51">
+      <c r="AD33" s="117">
         <v>5.6908387560000002E-2</v>
       </c>
-      <c r="AE33" s="51">
+      <c r="AE33" s="117">
         <v>3.6486215439999997E-2</v>
       </c>
-      <c r="AF33" s="59">
+      <c r="AF33" s="118">
         <v>0.5</v>
       </c>
-      <c r="AG33" s="51">
+      <c r="AG33" s="117">
         <v>0.22306052859442299</v>
       </c>
-      <c r="AH33" s="51">
+      <c r="AH33" s="117">
         <v>0.57247079603464301</v>
       </c>
-      <c r="AI33" s="59">
+      <c r="AI33" s="118">
         <v>0.5</v>
       </c>
     </row>
@@ -45032,25 +45089,25 @@
       <c r="Z34" s="40"/>
       <c r="AA34" s="40"/>
       <c r="AB34" s="40"/>
-      <c r="AC34" s="108" t="s">
+      <c r="AC34" s="119" t="s">
         <v>49</v>
       </c>
-      <c r="AD34" s="48">
+      <c r="AD34" s="120">
         <v>9.4283246605142298E-2</v>
       </c>
-      <c r="AE34" s="48">
+      <c r="AE34" s="120">
         <v>0.19932026734902</v>
       </c>
-      <c r="AF34" s="57">
+      <c r="AF34" s="121">
         <v>0.71499999999999997</v>
       </c>
-      <c r="AG34" s="48">
+      <c r="AG34" s="120">
         <v>0.53968205047320095</v>
       </c>
-      <c r="AH34" s="48">
+      <c r="AH34" s="120">
         <v>1.1832514378477199</v>
       </c>
-      <c r="AI34" s="57">
+      <c r="AI34" s="121">
         <v>0.63049999999999995</v>
       </c>
     </row>
@@ -45108,25 +45165,25 @@
       <c r="Z35" s="40"/>
       <c r="AA35" s="40"/>
       <c r="AB35" s="40"/>
-      <c r="AC35" s="108" t="s">
+      <c r="AC35" s="119" t="s">
         <v>50</v>
       </c>
-      <c r="AD35" s="48">
+      <c r="AD35" s="120">
         <v>8.8007029921725599E-2</v>
       </c>
-      <c r="AE35" s="48">
+      <c r="AE35" s="120">
         <v>0.190747163168177</v>
       </c>
-      <c r="AF35" s="57">
+      <c r="AF35" s="121">
         <v>0.71319999999999995</v>
       </c>
-      <c r="AG35" s="48">
+      <c r="AG35" s="120">
         <v>0.45501519469798102</v>
       </c>
-      <c r="AH35" s="48">
+      <c r="AH35" s="120">
         <v>1.0246348663465901</v>
       </c>
-      <c r="AI35" s="57">
+      <c r="AI35" s="121">
         <v>0.63039999999999996</v>
       </c>
     </row>
@@ -45184,25 +45241,25 @@
       <c r="Z36" s="40"/>
       <c r="AA36" s="40"/>
       <c r="AB36" s="40"/>
-      <c r="AC36" s="108" t="s">
+      <c r="AC36" s="119" t="s">
         <v>51</v>
       </c>
-      <c r="AD36" s="48">
+      <c r="AD36" s="120">
         <v>0.30389051417097901</v>
       </c>
-      <c r="AE36" s="48">
+      <c r="AE36" s="120">
         <v>0.63120965714843202</v>
       </c>
-      <c r="AF36" s="80">
+      <c r="AF36" s="128">
         <v>0.71679999999999999</v>
       </c>
-      <c r="AG36" s="48">
+      <c r="AG36" s="120">
         <v>0.46698380202338502</v>
       </c>
-      <c r="AH36" s="48">
+      <c r="AH36" s="120">
         <v>1.0579946893515</v>
       </c>
-      <c r="AI36" s="57">
+      <c r="AI36" s="121">
         <v>0.63129999999999997</v>
       </c>
     </row>
@@ -45249,25 +45306,25 @@
       <c r="O37" s="57">
         <v>0.71499999999999997</v>
       </c>
-      <c r="AC37" s="109" t="s">
+      <c r="AC37" s="122" t="s">
         <v>71</v>
       </c>
-      <c r="AD37" s="69">
+      <c r="AD37" s="123">
         <v>6.3393036829999999E-2</v>
       </c>
-      <c r="AE37" s="69">
+      <c r="AE37" s="123">
         <v>4.1257850950000001E-2</v>
       </c>
-      <c r="AF37" s="70">
+      <c r="AF37" s="124">
         <v>0.5</v>
       </c>
-      <c r="AG37" s="69">
+      <c r="AG37" s="123">
         <v>0.20240815556369701</v>
       </c>
-      <c r="AH37" s="69">
+      <c r="AH37" s="123">
         <v>0.51803475107129804</v>
       </c>
-      <c r="AI37" s="70">
+      <c r="AI37" s="124">
         <v>0.5</v>
       </c>
     </row>
@@ -45314,25 +45371,25 @@
       <c r="O38" s="57">
         <v>0.71319999999999995</v>
       </c>
-      <c r="AC38" s="108" t="s">
+      <c r="AC38" s="119" t="s">
         <v>72</v>
       </c>
-      <c r="AD38" s="48">
+      <c r="AD38" s="120">
         <v>0.28173425680133901</v>
       </c>
-      <c r="AE38" s="48">
+      <c r="AE38" s="120">
         <v>0.58945529813573005</v>
       </c>
-      <c r="AF38" s="57">
+      <c r="AF38" s="121">
         <v>0.71230000000000004</v>
       </c>
-      <c r="AG38" s="48">
+      <c r="AG38" s="120">
         <v>0.47297421949302298</v>
       </c>
-      <c r="AH38" s="48">
+      <c r="AH38" s="120">
         <v>1.0370412173102901</v>
       </c>
-      <c r="AI38" s="57">
+      <c r="AI38" s="121">
         <v>0.62619999999999998</v>
       </c>
     </row>
@@ -45379,25 +45436,25 @@
       <c r="O39" s="80">
         <v>0.71679999999999999</v>
       </c>
-      <c r="AC39" s="108" t="s">
+      <c r="AC39" s="119" t="s">
         <v>73</v>
       </c>
-      <c r="AD39" s="48">
+      <c r="AD39" s="120">
         <v>0.30598852213529798</v>
       </c>
-      <c r="AE39" s="48">
+      <c r="AE39" s="120">
         <v>0.62053947586219205</v>
       </c>
-      <c r="AF39" s="57">
+      <c r="AF39" s="121">
         <v>0.7077</v>
       </c>
-      <c r="AG39" s="48">
+      <c r="AG39" s="120">
         <v>0.52561685564685801</v>
       </c>
-      <c r="AH39" s="48">
+      <c r="AH39" s="120">
         <v>1.1852013775805299</v>
       </c>
-      <c r="AI39" s="57">
+      <c r="AI39" s="121">
         <v>0.63380000000000003</v>
       </c>
     </row>
@@ -45444,25 +45501,25 @@
       <c r="O40" s="70">
         <v>0.5</v>
       </c>
-      <c r="AC40" s="112" t="s">
+      <c r="AC40" s="129" t="s">
         <v>74</v>
       </c>
-      <c r="AD40" s="73">
+      <c r="AD40" s="130">
         <v>0.30939914773180999</v>
       </c>
-      <c r="AE40" s="73">
+      <c r="AE40" s="130">
         <v>0.65151138345691895</v>
       </c>
-      <c r="AF40" s="60">
+      <c r="AF40" s="131">
         <v>0.70899999999999996</v>
       </c>
-      <c r="AG40" s="73">
+      <c r="AG40" s="130">
         <v>0.57279847152926999</v>
       </c>
-      <c r="AH40" s="73">
+      <c r="AH40" s="130">
         <v>1.26618403019026</v>
       </c>
-      <c r="AI40" s="79">
+      <c r="AI40" s="132">
         <v>0.64700000000000002</v>
       </c>
     </row>
@@ -45599,21 +45656,21 @@
       </c>
     </row>
     <row r="45" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="C45" s="105" t="s">
+      <c r="C45" s="104" t="s">
         <v>56</v>
       </c>
-      <c r="D45" s="105"/>
-      <c r="E45" s="105"/>
-      <c r="F45" s="105"/>
-      <c r="G45" s="105"/>
-      <c r="H45" s="105"/>
-      <c r="I45" s="105"/>
-      <c r="J45" s="105"/>
-      <c r="K45" s="105"/>
-      <c r="L45" s="105"/>
-      <c r="M45" s="105"/>
-      <c r="N45" s="105"/>
-      <c r="O45" s="105"/>
+      <c r="D45" s="104"/>
+      <c r="E45" s="104"/>
+      <c r="F45" s="104"/>
+      <c r="G45" s="104"/>
+      <c r="H45" s="104"/>
+      <c r="I45" s="104"/>
+      <c r="J45" s="104"/>
+      <c r="K45" s="104"/>
+      <c r="L45" s="104"/>
+      <c r="M45" s="104"/>
+      <c r="N45" s="104"/>
+      <c r="O45" s="104"/>
     </row>
     <row r="46" spans="2:35" x14ac:dyDescent="0.2">
       <c r="C46" s="86" t="s">
@@ -45704,19 +45761,19 @@
       <c r="B48" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C48" s="102"/>
-      <c r="D48" s="103"/>
-      <c r="E48" s="103"/>
-      <c r="F48" s="103"/>
-      <c r="G48" s="103"/>
-      <c r="H48" s="103"/>
-      <c r="I48" s="103"/>
-      <c r="J48" s="103"/>
-      <c r="K48" s="103"/>
-      <c r="L48" s="103"/>
-      <c r="M48" s="103"/>
-      <c r="N48" s="103"/>
-      <c r="O48" s="104"/>
+      <c r="C48" s="101"/>
+      <c r="D48" s="102"/>
+      <c r="E48" s="102"/>
+      <c r="F48" s="102"/>
+      <c r="G48" s="102"/>
+      <c r="H48" s="102"/>
+      <c r="I48" s="102"/>
+      <c r="J48" s="102"/>
+      <c r="K48" s="102"/>
+      <c r="L48" s="102"/>
+      <c r="M48" s="102"/>
+      <c r="N48" s="102"/>
+      <c r="O48" s="103"/>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B49" s="41" t="s">
@@ -45895,7 +45952,7 @@
       </c>
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B53" s="118" t="s">
+      <c r="B53" s="106" t="s">
         <v>67</v>
       </c>
       <c r="C53" s="67">
@@ -46436,7 +46493,7 @@
     <mergeCell ref="C27:O27"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:C18">
-    <cfRule type="colorScale" priority="30">
+    <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -46444,7 +46501,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="136">
+    <cfRule type="colorScale" priority="144">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -46456,6 +46513,86 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D18">
+    <cfRule type="colorScale" priority="142">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:E18">
+    <cfRule type="colorScale" priority="141">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F18">
+    <cfRule type="colorScale" priority="140">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G18">
+    <cfRule type="colorScale" priority="139">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:H18">
+    <cfRule type="colorScale" priority="138">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3:I18">
+    <cfRule type="colorScale" priority="137">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:J18">
+    <cfRule type="colorScale" priority="136">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3:K18">
+    <cfRule type="colorScale" priority="135">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L3:L18">
     <cfRule type="colorScale" priority="134">
       <colorScale>
         <cfvo type="min"/>
@@ -46465,7 +46602,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E18">
+  <conditionalFormatting sqref="M3:M18">
     <cfRule type="colorScale" priority="133">
       <colorScale>
         <cfvo type="min"/>
@@ -46475,7 +46612,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F18">
+  <conditionalFormatting sqref="N3:N18">
     <cfRule type="colorScale" priority="132">
       <colorScale>
         <cfvo type="min"/>
@@ -46485,7 +46622,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G18">
+  <conditionalFormatting sqref="O3:O18">
     <cfRule type="colorScale" priority="131">
       <colorScale>
         <cfvo type="min"/>
@@ -46495,7 +46632,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:H18">
+  <conditionalFormatting sqref="P3:P18">
     <cfRule type="colorScale" priority="130">
       <colorScale>
         <cfvo type="min"/>
@@ -46505,7 +46642,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I18">
+  <conditionalFormatting sqref="Q3:Q18">
     <cfRule type="colorScale" priority="129">
       <colorScale>
         <cfvo type="min"/>
@@ -46515,7 +46652,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J18">
+  <conditionalFormatting sqref="R3:R18">
     <cfRule type="colorScale" priority="128">
       <colorScale>
         <cfvo type="min"/>
@@ -46525,7 +46662,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K18">
+  <conditionalFormatting sqref="S3:S18">
     <cfRule type="colorScale" priority="127">
       <colorScale>
         <cfvo type="min"/>
@@ -46535,7 +46672,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L3:L18">
+  <conditionalFormatting sqref="T3:T18">
     <cfRule type="colorScale" priority="126">
       <colorScale>
         <cfvo type="min"/>
@@ -46545,7 +46682,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M18">
+  <conditionalFormatting sqref="U3:U18">
     <cfRule type="colorScale" priority="125">
       <colorScale>
         <cfvo type="min"/>
@@ -46555,7 +46692,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3:N18">
+  <conditionalFormatting sqref="V3:V18">
     <cfRule type="colorScale" priority="124">
       <colorScale>
         <cfvo type="min"/>
@@ -46565,7 +46702,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O3:O18">
+  <conditionalFormatting sqref="W3:W18">
     <cfRule type="colorScale" priority="123">
       <colorScale>
         <cfvo type="min"/>
@@ -46575,7 +46712,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P18">
+  <conditionalFormatting sqref="X3:X18">
     <cfRule type="colorScale" priority="122">
       <colorScale>
         <cfvo type="min"/>
@@ -46585,7 +46722,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q3:Q18">
+  <conditionalFormatting sqref="Y3:Y18">
     <cfRule type="colorScale" priority="121">
       <colorScale>
         <cfvo type="min"/>
@@ -46595,7 +46732,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R3:R18">
+  <conditionalFormatting sqref="Z3:Z18">
     <cfRule type="colorScale" priority="120">
       <colorScale>
         <cfvo type="min"/>
@@ -46605,88 +46742,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S3:S18">
-    <cfRule type="colorScale" priority="119">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T3:T18">
-    <cfRule type="colorScale" priority="118">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="U3:U18">
-    <cfRule type="colorScale" priority="117">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V3:V18">
-    <cfRule type="colorScale" priority="116">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="W3:W18">
-    <cfRule type="colorScale" priority="115">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X3:X18">
-    <cfRule type="colorScale" priority="114">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y3:Y18">
-    <cfRule type="colorScale" priority="113">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Z3:Z18">
-    <cfRule type="colorScale" priority="112">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="O28:O43">
-    <cfRule type="colorScale" priority="99">
+    <cfRule type="colorScale" priority="107">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -46696,6 +46753,86 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L28:L43">
+    <cfRule type="colorScale" priority="84">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M28:M43">
+    <cfRule type="colorScale" priority="83">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N28:N43">
+    <cfRule type="colorScale" priority="82">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C28:C43">
+    <cfRule type="colorScale" priority="81">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D28:D43">
+    <cfRule type="colorScale" priority="80">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E28:E43">
+    <cfRule type="colorScale" priority="79">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F28:F43">
+    <cfRule type="colorScale" priority="78">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G28:G43">
+    <cfRule type="colorScale" priority="77">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H28:H43">
     <cfRule type="colorScale" priority="76">
       <colorScale>
         <cfvo type="min"/>
@@ -46705,7 +46842,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M28:M43">
+  <conditionalFormatting sqref="I28:I43">
     <cfRule type="colorScale" priority="75">
       <colorScale>
         <cfvo type="min"/>
@@ -46715,7 +46852,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N28:N43">
+  <conditionalFormatting sqref="J28:J43">
     <cfRule type="colorScale" priority="74">
       <colorScale>
         <cfvo type="min"/>
@@ -46725,7 +46862,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C28:C43">
+  <conditionalFormatting sqref="K28:K43">
     <cfRule type="colorScale" priority="73">
       <colorScale>
         <cfvo type="min"/>
@@ -46735,8 +46872,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D28:D43">
-    <cfRule type="colorScale" priority="72">
+  <conditionalFormatting sqref="O49:O64">
+    <cfRule type="colorScale" priority="51">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -46745,8 +46882,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E28:E43">
-    <cfRule type="colorScale" priority="71">
+  <conditionalFormatting sqref="L49:L64">
+    <cfRule type="colorScale" priority="50">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -46755,8 +46892,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F28:F43">
-    <cfRule type="colorScale" priority="70">
+  <conditionalFormatting sqref="M49:M64">
+    <cfRule type="colorScale" priority="49">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -46765,8 +46902,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G28:G43">
-    <cfRule type="colorScale" priority="69">
+  <conditionalFormatting sqref="N49:N64">
+    <cfRule type="colorScale" priority="48">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -46775,8 +46912,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H28:H43">
-    <cfRule type="colorScale" priority="68">
+  <conditionalFormatting sqref="C49:C64">
+    <cfRule type="colorScale" priority="47">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -46785,8 +46922,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I28:I43">
-    <cfRule type="colorScale" priority="67">
+  <conditionalFormatting sqref="D49:D64">
+    <cfRule type="colorScale" priority="46">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -46795,8 +46932,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J28:J43">
-    <cfRule type="colorScale" priority="66">
+  <conditionalFormatting sqref="E49:E64">
+    <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -46805,8 +46942,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K28:K43">
-    <cfRule type="colorScale" priority="65">
+  <conditionalFormatting sqref="F49:F64">
+    <cfRule type="colorScale" priority="44">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -46815,7 +46952,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O49:O64">
+  <conditionalFormatting sqref="G49:G64">
     <cfRule type="colorScale" priority="43">
       <colorScale>
         <cfvo type="min"/>
@@ -46825,7 +46962,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L49:L64">
+  <conditionalFormatting sqref="H49:H64">
     <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="min"/>
@@ -46835,7 +46972,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M49:M64">
+  <conditionalFormatting sqref="I49:I64">
     <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="min"/>
@@ -46845,7 +46982,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N49:N64">
+  <conditionalFormatting sqref="J49:J64">
     <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="min"/>
@@ -46855,7 +46992,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C64">
+  <conditionalFormatting sqref="K49:K64">
     <cfRule type="colorScale" priority="39">
       <colorScale>
         <cfvo type="min"/>
@@ -46865,17 +47002,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D49:D64">
-    <cfRule type="colorScale" priority="38">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E49:E64">
+  <conditionalFormatting sqref="AF25:AF40">
     <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="min"/>
@@ -46885,57 +47012,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F49:F64">
-    <cfRule type="colorScale" priority="36">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G49:G64">
-    <cfRule type="colorScale" priority="35">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H49:H64">
-    <cfRule type="colorScale" priority="34">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I49:I64">
-    <cfRule type="colorScale" priority="33">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J49:J64">
-    <cfRule type="colorScale" priority="32">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K49:K64">
+  <conditionalFormatting sqref="AD25:AD40">
     <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
@@ -46945,28 +47022,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF25:AF40">
-    <cfRule type="colorScale" priority="29">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD25:AD40">
-    <cfRule type="colorScale" priority="23">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="AE25:AE40">
-    <cfRule type="colorScale" priority="20">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -46976,7 +47033,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI25:AI40">
-    <cfRule type="colorScale" priority="3">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -46986,7 +47043,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG25:AG40">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -46996,12 +47053,80 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH25:AH40">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
         <color rgb="FFFCFCFF"/>
         <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD24:AD40">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="0"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE24:AE40">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="0"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF24:AF40">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="0"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG24:AG40">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="0"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH24:AH40">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="0"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="0"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI24:AI40">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="0"/>
+        <color rgb="FFFFEF9C"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
@@ -47040,38 +47165,38 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="29"/>
-      <c r="B1" s="106" t="s">
+      <c r="B1" s="105" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106" t="s">
+      <c r="C1" s="105"/>
+      <c r="D1" s="105" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106" t="s">
+      <c r="E1" s="105"/>
+      <c r="F1" s="105" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="106"/>
-      <c r="H1" s="106" t="s">
+      <c r="G1" s="105"/>
+      <c r="H1" s="105" t="s">
         <v>60</v>
       </c>
-      <c r="I1" s="106"/>
-      <c r="J1" s="106" t="s">
+      <c r="I1" s="105"/>
+      <c r="J1" s="105" t="s">
         <v>61</v>
       </c>
-      <c r="K1" s="106"/>
-      <c r="L1" s="106" t="s">
+      <c r="K1" s="105"/>
+      <c r="L1" s="105" t="s">
         <v>49</v>
       </c>
-      <c r="M1" s="106"/>
-      <c r="N1" s="106" t="s">
+      <c r="M1" s="105"/>
+      <c r="N1" s="105" t="s">
         <v>50</v>
       </c>
-      <c r="O1" s="106"/>
-      <c r="P1" s="106" t="s">
+      <c r="O1" s="105"/>
+      <c r="P1" s="105" t="s">
         <v>51</v>
       </c>
-      <c r="Q1" s="106"/>
+      <c r="Q1" s="105"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="29"/>
@@ -47242,7 +47367,7 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A11" s="98" t="s">
+      <c r="A11" s="97" t="s">
         <v>57</v>
       </c>
       <c r="B11" s="10" t="s">
@@ -47257,7 +47382,7 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A12" s="99"/>
+      <c r="A12" s="98"/>
       <c r="B12" s="11" t="s">
         <v>45</v>
       </c>
@@ -47281,7 +47406,7 @@
       <c r="Q12" s="39"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A13" s="99"/>
+      <c r="A13" s="98"/>
       <c r="B13" s="11" t="s">
         <v>46</v>
       </c>
@@ -47305,7 +47430,7 @@
       <c r="Q13" s="39"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A14" s="99"/>
+      <c r="A14" s="98"/>
       <c r="B14" s="12" t="s">
         <v>47</v>
       </c>
@@ -47329,7 +47454,7 @@
       <c r="Q14" s="39"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A15" s="99"/>
+      <c r="A15" s="98"/>
       <c r="B15" s="10" t="s">
         <v>48</v>
       </c>
@@ -47353,7 +47478,7 @@
       <c r="Q15" s="39"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A16" s="99"/>
+      <c r="A16" s="98"/>
       <c r="B16" s="11" t="s">
         <v>49</v>
       </c>
@@ -47377,7 +47502,7 @@
       <c r="Q16" s="39"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A17" s="99"/>
+      <c r="A17" s="98"/>
       <c r="B17" s="11" t="s">
         <v>50</v>
       </c>
@@ -47401,7 +47526,7 @@
       <c r="Q17" s="39"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A18" s="99"/>
+      <c r="A18" s="98"/>
       <c r="B18" s="12" t="s">
         <v>51</v>
       </c>
@@ -47425,7 +47550,7 @@
       <c r="Q18" s="39"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A19" s="100" t="s">
+      <c r="A19" s="99" t="s">
         <v>58</v>
       </c>
       <c r="B19" s="10" t="s">
@@ -47451,7 +47576,7 @@
       <c r="Q19" s="39"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A20" s="99"/>
+      <c r="A20" s="98"/>
       <c r="B20" s="11" t="s">
         <v>68</v>
       </c>
@@ -47475,7 +47600,7 @@
       <c r="Q20" s="39"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A21" s="99"/>
+      <c r="A21" s="98"/>
       <c r="B21" s="11" t="s">
         <v>69</v>
       </c>
@@ -47499,7 +47624,7 @@
       <c r="Q21" s="39"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A22" s="99"/>
+      <c r="A22" s="98"/>
       <c r="B22" s="12" t="s">
         <v>70</v>
       </c>
@@ -47523,7 +47648,7 @@
       <c r="Q22" s="39"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A23" s="99"/>
+      <c r="A23" s="98"/>
       <c r="B23" s="10" t="s">
         <v>71</v>
       </c>
@@ -47547,7 +47672,7 @@
       <c r="Q23" s="39"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A24" s="99"/>
+      <c r="A24" s="98"/>
       <c r="B24" s="11" t="s">
         <v>72</v>
       </c>
@@ -47571,7 +47696,7 @@
       <c r="Q24" s="39"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A25" s="99"/>
+      <c r="A25" s="98"/>
       <c r="B25" s="11" t="s">
         <v>73</v>
       </c>
@@ -47595,7 +47720,7 @@
       <c r="Q25" s="39"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A26" s="101"/>
+      <c r="A26" s="100"/>
       <c r="B26" s="12" t="s">
         <v>74</v>
       </c>

</xml_diff>